<commit_message>
Update Nydar loc GLM composite.xlsx
</commit_message>
<xml_diff>
--- a/Mosquito Life history colab/Life history local/GLMs/Nydar loc GLM composite.xlsx
+++ b/Mosquito Life history colab/Life history local/GLMs/Nydar loc GLM composite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Documents\GitHub\wingproj\Mosquito Life history colab\Life history local\GLMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{96403234-671A-446D-ACD3-ACAFCBD346CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2153A07-7F4E-4483-84A8-333E59080790}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Used for report" sheetId="10" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6993" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6985" uniqueCount="645">
   <si>
     <t>[1]</t>
   </si>
@@ -2846,7 +2846,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2859,9 +2859,6 @@
     </xf>
     <xf numFmtId="16" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2980,15 +2977,6 @@
     <xf numFmtId="2" fontId="21" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3054,15 +3042,6 @@
     <xf numFmtId="11" fontId="18" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="21" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3082,6 +3061,28 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3439,24 +3440,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E73D8F-CC79-4F3E-B18A-0D4B9A0F8849}">
   <dimension ref="A2:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:N28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3467,1084 +3468,1084 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="79" t="s">
         <v>643</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="86" t="s">
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="79" t="s">
         <v>642</v>
       </c>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="86" t="s">
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="79" t="s">
         <v>644</v>
       </c>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="88"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="82" t="s">
         <v>624</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="37" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="36" t="s">
         <v>618</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="38" t="s">
         <v>621</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="39" t="s">
         <v>618</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="38" t="s">
         <v>621</v>
       </c>
-      <c r="K4" s="40" t="s">
+      <c r="K4" s="39" t="s">
         <v>618</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="38" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="83"/>
+      <c r="B5" s="33" t="s">
         <v>625</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="40">
         <v>2.8862169999999998</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>9.0749999999999997E-3</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>318.03399999999999</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>629</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="24">
         <v>4.66418</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="23">
         <v>6.8229999999999999E-2</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="23">
         <v>68.363</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="28">
         <v>1.0139069999999999</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="8">
         <v>3.875E-3</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="8">
         <v>261.64600000000002</v>
       </c>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="29" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="34" t="s">
+      <c r="A6" s="83"/>
+      <c r="B6" s="33" t="s">
         <v>622</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="40">
         <v>-0.157638</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>1.3943000000000001E-2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>-11.305999999999999</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>629</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="24">
         <v>-1.67899</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="23">
         <v>9.6310000000000007E-2</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="23">
         <v>-17.434000000000001</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="28">
         <v>-4.5236999999999999E-2</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="8">
         <v>5.6309999999999997E-3</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="8">
         <v>-8.0340000000000007</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="26">
         <v>2.8200000000000001E-15</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="83"/>
+      <c r="B7" s="33" t="s">
         <v>623</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="40">
         <v>-0.31301800000000002</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>1.5528E-2</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>-20.158000000000001</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="25" t="s">
         <v>629</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="24">
         <v>-2.6410999999999998</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="23">
         <v>9.7229999999999997E-2</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="23">
         <v>-27.164999999999999</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7" s="28">
         <v>-8.2936999999999997E-2</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="8">
         <v>5.7460000000000002E-3</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="8">
         <v>-14.433999999999999</v>
       </c>
-      <c r="N7" s="30" t="s">
+      <c r="N7" s="29" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="33" t="s">
         <v>626</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="41">
         <v>4.3493999999999998E-2</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>1.1552E-2</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>3.7650000000000001</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>1.7699999999999999E-4</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="24">
         <v>9.8449999999999996E-2</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="23">
         <v>8.8349999999999998E-2</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="23">
         <v>1.1140000000000001</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="30">
         <v>0.26500000000000001</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K8" s="28">
         <v>4.7609999999999996E-3</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="8">
         <v>5.0400000000000002E-3</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="8">
         <v>0.94499999999999995</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="27">
         <v>0.34511700000000001</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="35" t="s">
+      <c r="A9" s="83"/>
+      <c r="B9" s="34" t="s">
         <v>627</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="41">
         <v>9.9410000000000002E-3</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>1.7724E-2</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>0.56100000000000005</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="27">
         <v>0.57501500000000005</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="24">
         <v>-0.25535000000000002</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="23">
         <v>0.12479999999999999</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="23">
         <v>-2.0459999999999998</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="31">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="28">
         <v>-2.4868999999999999E-2</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <v>7.3429999999999997E-3</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="8">
         <v>-3.387</v>
       </c>
-      <c r="N9" s="27">
+      <c r="N9" s="26">
         <v>7.3700000000000002E-4</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="36" t="s">
+      <c r="A10" s="84"/>
+      <c r="B10" s="35" t="s">
         <v>628</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="42">
         <v>3.1896000000000001E-2</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="43">
         <v>1.9782999999999999E-2</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E10" s="44">
         <v>1.6120000000000001</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="45">
         <v>0.107237</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="46">
         <v>-0.11594</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="47">
         <v>0.12684000000000001</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="47">
         <v>-0.91400000000000003</v>
       </c>
-      <c r="J10" s="49">
+      <c r="J10" s="48">
         <v>0.36099999999999999</v>
       </c>
-      <c r="K10" s="50">
+      <c r="K10" s="49">
         <v>-5.2760000000000003E-3</v>
       </c>
-      <c r="L10" s="45">
+      <c r="L10" s="44">
         <v>7.541E-3</v>
       </c>
-      <c r="M10" s="45">
+      <c r="M10" s="44">
         <v>-0.7</v>
       </c>
-      <c r="N10" s="46">
+      <c r="N10" s="45">
         <v>0.48430499999999999</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="82" t="s">
         <v>630</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="40" t="s">
+      <c r="B11" s="59"/>
+      <c r="C11" s="39" t="s">
         <v>618</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="52" t="s">
         <v>621</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="36" t="s">
         <v>618</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="I11" s="38" t="s">
+      <c r="I11" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="38" t="s">
         <v>621</v>
       </c>
-      <c r="K11" s="61" t="s">
+      <c r="K11" s="57" t="s">
         <v>618</v>
       </c>
-      <c r="L11" s="54" t="s">
+      <c r="L11" s="50" t="s">
         <v>619</v>
       </c>
-      <c r="M11" s="54" t="s">
+      <c r="M11" s="50" t="s">
         <v>620</v>
       </c>
-      <c r="N11" s="55" t="s">
+      <c r="N11" s="51" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="64" t="s">
+      <c r="A12" s="83"/>
+      <c r="B12" s="60" t="s">
         <v>631</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="28">
         <v>3.0078140000000002</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>8.1779999999999995E-3</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>367.78</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="53" t="s">
         <v>629</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="40">
         <v>4.1160220000000001</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>6.0004000000000002E-2</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <v>68.596000000000004</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="25" t="s">
         <v>425</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="28">
         <v>1.0309026999999999</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="8">
         <v>3.5241000000000001E-3</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="8">
         <v>292.529</v>
       </c>
-      <c r="N12" s="26" t="s">
+      <c r="N12" s="25" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="64" t="s">
+      <c r="A13" s="83"/>
+      <c r="B13" s="60" t="s">
         <v>622</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <v>-0.182947</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>1.2718E-2</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>-14.385</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="53" t="s">
         <v>629</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="40">
         <v>-1.338848</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>8.4511000000000003E-2</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <v>-15.842000000000001</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="25" t="s">
         <v>425</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="28">
         <v>-5.9019599999999998E-2</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="8">
         <v>5.1224E-3</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="8">
         <v>-11.522</v>
       </c>
-      <c r="N13" s="26" t="s">
+      <c r="N13" s="25" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="64" t="s">
+      <c r="A14" s="83"/>
+      <c r="B14" s="60" t="s">
         <v>623</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>-0.25945200000000002</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>1.4531000000000001E-2</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>-17.855</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="53" t="s">
         <v>629</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="40">
         <v>-2.3713410000000001</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>9.0676999999999994E-2</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="8">
         <v>-26.152000000000001</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="25" t="s">
         <v>425</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="28">
         <v>-0.11669350000000001</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="8">
         <v>5.7399E-3</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="8">
         <v>-20.329999999999998</v>
       </c>
-      <c r="N14" s="26" t="s">
+      <c r="N14" s="25" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="64" t="s">
+      <c r="A15" s="83"/>
+      <c r="B15" s="60" t="s">
         <v>632</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="28">
         <v>5.8056999999999997E-2</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>1.1091999999999999E-2</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>5.234</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="54">
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="40">
         <v>-1.439E-3</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>8.3634E-2</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="8">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="27">
         <v>0.98629999999999995</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="28">
         <v>9.2230000000000003E-4</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="8">
         <v>4.9148999999999998E-3</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="8">
         <v>0.188</v>
       </c>
-      <c r="N15" s="28">
+      <c r="N15" s="27">
         <v>0.85099999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="65" t="s">
+      <c r="A16" s="83"/>
+      <c r="B16" s="61" t="s">
         <v>633</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="28">
         <v>-3.3419999999999998E-2</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>1.7385000000000001E-2</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>-1.9219999999999999</v>
       </c>
-      <c r="F16" s="59">
+      <c r="F16" s="55">
         <v>5.4826E-2</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="40">
         <v>0.22934099999999999</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <v>0.117662</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="8">
         <v>1.9490000000000001</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="27">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="28">
         <v>2.6613000000000001E-3</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="8">
         <v>7.1301999999999997E-3</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="8">
         <v>0.373</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="27">
         <v>0.70899999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="53"/>
-      <c r="B17" s="66" t="s">
+      <c r="A17" s="84"/>
+      <c r="B17" s="62" t="s">
         <v>634</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="49">
         <v>-6.8000000000000005E-2</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="43">
         <v>1.9924000000000001E-2</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="44">
         <v>-3.4129999999999998</v>
       </c>
-      <c r="F17" s="60">
+      <c r="F17" s="56">
         <v>6.6699999999999995E-4</v>
       </c>
-      <c r="G17" s="62">
+      <c r="G17" s="58">
         <v>-1.8242000000000001E-2</v>
       </c>
-      <c r="H17" s="45">
+      <c r="H17" s="44">
         <v>0.12525700000000001</v>
       </c>
-      <c r="I17" s="45">
+      <c r="I17" s="44">
         <v>-0.14599999999999999</v>
       </c>
-      <c r="J17" s="46">
+      <c r="J17" s="45">
         <v>0.88419999999999999</v>
       </c>
-      <c r="K17" s="50">
+      <c r="K17" s="49">
         <v>9.1874999999999995E-3</v>
       </c>
-      <c r="L17" s="45">
+      <c r="L17" s="44">
         <v>7.8951999999999998E-3</v>
       </c>
-      <c r="M17" s="45">
+      <c r="M17" s="44">
         <v>1.1639999999999999</v>
       </c>
-      <c r="N17" s="46">
+      <c r="N17" s="45">
         <v>0.245</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="82" t="s">
         <v>635</v>
       </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="37" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="36" t="s">
         <v>618</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="38" t="s">
         <v>621</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="39" t="s">
         <v>618</v>
       </c>
-      <c r="H18" s="38" t="s">
+      <c r="H18" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="J18" s="56" t="s">
+      <c r="J18" s="52" t="s">
         <v>621</v>
       </c>
-      <c r="K18" s="73" t="s">
+      <c r="K18" s="69" t="s">
         <v>618</v>
       </c>
-      <c r="L18" s="54" t="s">
+      <c r="L18" s="50" t="s">
         <v>619</v>
       </c>
-      <c r="M18" s="54" t="s">
+      <c r="M18" s="50" t="s">
         <v>620</v>
       </c>
-      <c r="N18" s="55" t="s">
+      <c r="N18" s="51" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="69" t="s">
+      <c r="A19" s="83"/>
+      <c r="B19" s="65" t="s">
         <v>636</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="40">
         <v>3.0543089999999999</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>1.1594999999999999E-2</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>263.41899999999998</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="25" t="s">
         <v>629</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="28">
         <v>3.46739</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>6.6019999999999995E-2</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="8">
         <v>52.518999999999998</v>
       </c>
-      <c r="J19" s="57" t="s">
+      <c r="J19" s="53" t="s">
         <v>425</v>
       </c>
-      <c r="K19" s="41">
+      <c r="K19" s="40">
         <v>1.022661</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="8">
         <v>4.6639999999999997E-3</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="8">
         <v>219.27</v>
       </c>
-      <c r="N19" s="26" t="s">
+      <c r="N19" s="25" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
-      <c r="B20" s="69" t="s">
+      <c r="A20" s="83"/>
+      <c r="B20" s="65" t="s">
         <v>622</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="40">
         <v>-0.102379</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>1.7752E-2</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>-5.7670000000000003</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="26">
         <v>1.85E-8</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="28">
         <v>-1.16977</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>9.5570000000000002E-2</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>-12.241</v>
       </c>
-      <c r="J20" s="57" t="s">
+      <c r="J20" s="53" t="s">
         <v>425</v>
       </c>
-      <c r="K20" s="41">
+      <c r="K20" s="40">
         <v>-2.8965000000000001E-2</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <v>6.8840000000000004E-3</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="8">
         <v>-4.2069999999999999</v>
       </c>
-      <c r="N20" s="27">
+      <c r="N20" s="26">
         <v>3.3599999999999997E-5</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="69" t="s">
+      <c r="A21" s="83"/>
+      <c r="B21" s="65" t="s">
         <v>623</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="40">
         <v>-0.209563</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>1.9983999999999998E-2</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>-10.487</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="25" t="s">
         <v>629</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="28">
         <v>-1.6927399999999999</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>0.10002999999999999</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="8">
         <v>-16.922000000000001</v>
       </c>
-      <c r="J21" s="57" t="s">
+      <c r="J21" s="53" t="s">
         <v>425</v>
       </c>
-      <c r="K21" s="41">
+      <c r="K21" s="40">
         <v>-8.4042000000000006E-2</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="8">
         <v>7.4130000000000003E-3</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="8">
         <v>-11.337999999999999</v>
       </c>
-      <c r="N21" s="26" t="s">
+      <c r="N21" s="25" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="69" t="s">
+      <c r="A22" s="83"/>
+      <c r="B22" s="65" t="s">
         <v>637</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="40">
         <v>1.8095E-2</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>2.2522E-2</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>0.80300000000000005</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="27">
         <v>0.42230000000000001</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="28">
         <v>9.511E-2</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <v>0.12995999999999999</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="8">
         <v>0.73199999999999998</v>
       </c>
-      <c r="J22" s="59">
+      <c r="J22" s="55">
         <v>0.46500000000000002</v>
       </c>
-      <c r="K22" s="41">
+      <c r="K22" s="40">
         <v>2.2040000000000001E-2</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="8">
         <v>9.0279999999999996E-3</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="8">
         <v>2.4409999999999998</v>
       </c>
-      <c r="N22" s="67">
+      <c r="N22" s="63">
         <v>1.52E-2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="70" t="s">
+      <c r="A23" s="83"/>
+      <c r="B23" s="66" t="s">
         <v>638</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="40">
         <v>8.4159999999999999E-3</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>3.3154000000000003E-2</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>0.254</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="27">
         <v>0.79979999999999996</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="28">
         <v>3.5839999999999997E-2</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <v>0.18199000000000001</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="8">
         <v>0.19700000000000001</v>
       </c>
-      <c r="J23" s="59">
+      <c r="J23" s="55">
         <v>0.84399999999999997</v>
       </c>
-      <c r="K23" s="41">
+      <c r="K23" s="40">
         <v>1.0718E-2</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="8">
         <v>1.286E-2</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="8">
         <v>0.83299999999999996</v>
       </c>
-      <c r="N23" s="28">
+      <c r="N23" s="27">
         <v>0.4052</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="53"/>
-      <c r="B24" s="71" t="s">
+      <c r="A24" s="84"/>
+      <c r="B24" s="67" t="s">
         <v>639</v>
       </c>
-      <c r="C24" s="62">
+      <c r="C24" s="58">
         <v>6.8352999999999997E-2</v>
       </c>
-      <c r="D24" s="44">
+      <c r="D24" s="43">
         <v>3.7832999999999999E-2</v>
       </c>
-      <c r="E24" s="45">
+      <c r="E24" s="44">
         <v>1.8069999999999999</v>
       </c>
-      <c r="F24" s="46">
+      <c r="F24" s="45">
         <v>7.17E-2</v>
       </c>
-      <c r="G24" s="50">
+      <c r="G24" s="49">
         <v>0.21357999999999999</v>
       </c>
-      <c r="H24" s="45">
+      <c r="H24" s="44">
         <v>0.19811000000000001</v>
       </c>
-      <c r="I24" s="45">
+      <c r="I24" s="44">
         <v>1.0780000000000001</v>
       </c>
-      <c r="J24" s="72">
+      <c r="J24" s="68">
         <v>0.28199999999999997</v>
       </c>
-      <c r="K24" s="62">
+      <c r="K24" s="58">
         <v>2.2963000000000001E-2</v>
       </c>
-      <c r="L24" s="45">
+      <c r="L24" s="44">
         <v>1.421E-2</v>
       </c>
-      <c r="M24" s="45">
+      <c r="M24" s="44">
         <v>1.6160000000000001</v>
       </c>
-      <c r="N24" s="46">
+      <c r="N24" s="45">
         <v>0.1071</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="85" t="s">
         <v>640</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="40" t="s">
+      <c r="B25" s="32"/>
+      <c r="C25" s="39" t="s">
         <v>618</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="F25" s="56" t="s">
+      <c r="F25" s="52" t="s">
         <v>621</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="36" t="s">
         <v>618</v>
       </c>
-      <c r="H25" s="38" t="s">
+      <c r="H25" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="I25" s="38" t="s">
+      <c r="I25" s="37" t="s">
         <v>620</v>
       </c>
-      <c r="J25" s="39" t="s">
+      <c r="J25" s="38" t="s">
         <v>621</v>
       </c>
-      <c r="K25" s="61" t="s">
+      <c r="K25" s="57" t="s">
         <v>618</v>
       </c>
-      <c r="L25" s="54" t="s">
+      <c r="L25" s="50" t="s">
         <v>619</v>
       </c>
-      <c r="M25" s="54" t="s">
+      <c r="M25" s="50" t="s">
         <v>620</v>
       </c>
-      <c r="N25" s="55" t="s">
+      <c r="N25" s="51" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="78"/>
-      <c r="B26" s="34" t="s">
+      <c r="A26" s="86"/>
+      <c r="B26" s="33" t="s">
         <v>641</v>
       </c>
-      <c r="C26" s="80">
+      <c r="C26" s="73">
         <v>3.15</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="15">
         <v>3.3529999999999997E-2</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="16">
         <v>93.944000000000003</v>
       </c>
-      <c r="F26" s="83">
+      <c r="F26" s="76">
         <v>2E-16</v>
       </c>
-      <c r="G26" s="41">
+      <c r="G26" s="40">
         <v>4.8</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="8">
         <v>0.20813000000000001</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="8">
         <v>23.062000000000001</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="25" t="s">
         <v>629</v>
       </c>
-      <c r="K26" s="29">
+      <c r="K26" s="28">
         <v>1.0675589999999999</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="8">
         <v>1.1812E-2</v>
       </c>
-      <c r="M26" s="9">
+      <c r="M26" s="8">
         <v>90.376000000000005</v>
       </c>
-      <c r="N26" s="26" t="s">
+      <c r="N26" s="25" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="78"/>
-      <c r="B27" s="34" t="s">
+      <c r="A27" s="86"/>
+      <c r="B27" s="33" t="s">
         <v>622</v>
       </c>
-      <c r="C27" s="80">
+      <c r="C27" s="73">
         <v>-0.25209999999999999</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="15">
         <v>5.1119999999999999E-2</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="16">
         <v>-4.9320000000000004</v>
       </c>
-      <c r="F27" s="83">
+      <c r="F27" s="76">
         <v>1.4699999999999999E-6</v>
       </c>
-      <c r="G27" s="41">
+      <c r="G27" s="40">
         <v>-1.8714299999999999</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="8">
         <v>0.27250999999999997</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="8">
         <v>-6.867</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J27" s="26">
         <v>2.78E-11</v>
       </c>
-      <c r="K27" s="29">
+      <c r="K27" s="28">
         <v>-5.8819999999999997E-2</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="8">
         <v>1.6213000000000002E-2</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="8">
         <v>-3.6280000000000001</v>
       </c>
-      <c r="N27" s="27">
+      <c r="N27" s="26">
         <v>3.4699999999999998E-4</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="79"/>
-      <c r="B28" s="82" t="s">
+      <c r="A28" s="87"/>
+      <c r="B28" s="75" t="s">
         <v>623</v>
       </c>
-      <c r="C28" s="81">
+      <c r="C28" s="74">
         <v>-0.33150000000000002</v>
       </c>
-      <c r="D28" s="74">
+      <c r="D28" s="70">
         <v>8.7569999999999995E-2</v>
       </c>
-      <c r="E28" s="75">
+      <c r="E28" s="71">
         <v>-3.7850000000000001</v>
       </c>
-      <c r="F28" s="84">
+      <c r="F28" s="77">
         <v>1.92E-4</v>
       </c>
-      <c r="G28" s="62">
+      <c r="G28" s="58">
         <v>-2.7285699999999999</v>
       </c>
-      <c r="H28" s="45">
+      <c r="H28" s="44">
         <v>0.27250999999999997</v>
       </c>
-      <c r="I28" s="45">
+      <c r="I28" s="44">
         <v>-10.013</v>
       </c>
-      <c r="J28" s="85" t="s">
+      <c r="J28" s="78" t="s">
         <v>629</v>
       </c>
-      <c r="K28" s="50">
+      <c r="K28" s="49">
         <v>-8.2863000000000006E-2</v>
       </c>
-      <c r="L28" s="45">
+      <c r="L28" s="44">
         <v>2.4340000000000001E-2</v>
       </c>
-      <c r="M28" s="45">
+      <c r="M28" s="44">
         <v>-3.4039999999999999</v>
       </c>
-      <c r="N28" s="76">
+      <c r="N28" s="72">
         <v>7.7399999999999995E-4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A25:A28"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A25:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13281,65 +13282,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AB33"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4:AB31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" activeCellId="3" sqref="M5:M7 M13:M15 M18 M21:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="8"/>
-    <col min="9" max="9" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="8"/>
-    <col min="16" max="16" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="9.140625" style="8"/>
-    <col min="24" max="24" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="7"/>
+    <col min="9" max="9" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="7"/>
+    <col min="16" max="16" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="9.140625" style="7"/>
+    <col min="24" max="24" width="20.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="88" t="s">
         <v>614</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="I2" s="88" t="s">
         <v>615</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7" t="s">
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88" t="s">
         <v>616</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
       <c r="V2" s="3"/>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="88" t="s">
         <v>617</v>
       </c>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="88"/>
+      <c r="Z2" s="88"/>
+      <c r="AA2" s="88"/>
+      <c r="AB2" s="88"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -13407,67 +13408,67 @@
       <c r="B5" s="5" t="s">
         <v>625</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>2.8862169999999998</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>9.0749999999999997E-3</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>318.03399999999999</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>625</v>
       </c>
-      <c r="J5" s="12">
-        <v>2.8862169999999998</v>
-      </c>
-      <c r="K5" s="13">
-        <v>9.0749999999999997E-3</v>
-      </c>
-      <c r="L5" s="12">
-        <v>318.03399999999999</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N5" s="8" t="s">
+      <c r="J5">
+        <v>1.057998</v>
+      </c>
+      <c r="K5">
+        <v>1.3141E-2</v>
+      </c>
+      <c r="L5">
+        <v>80.513999999999996</v>
+      </c>
+      <c r="M5" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>625</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="Q5" s="21">
         <v>4.66418</v>
       </c>
-      <c r="R5" s="22">
+      <c r="R5" s="21">
         <v>6.8229999999999999E-2</v>
       </c>
-      <c r="S5" s="22">
+      <c r="S5" s="21">
         <v>68.363</v>
       </c>
-      <c r="T5" s="21" t="s">
+      <c r="T5" s="20" t="s">
         <v>425</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>625</v>
       </c>
-      <c r="Y5" s="12">
+      <c r="Y5" s="11">
         <v>1.0139069999999999</v>
       </c>
-      <c r="Z5" s="12">
+      <c r="Z5" s="11">
         <v>3.875E-3</v>
       </c>
-      <c r="AA5" s="12">
+      <c r="AA5" s="11">
         <v>261.64600000000002</v>
       </c>
-      <c r="AB5" s="21" t="s">
+      <c r="AB5" s="20" t="s">
         <v>425</v>
       </c>
     </row>
@@ -13475,67 +13476,67 @@
       <c r="B6" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>-0.157638</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>1.3943000000000001E-2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>-11.305999999999999</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="J6" s="12">
-        <v>-0.157638</v>
-      </c>
-      <c r="K6" s="13">
-        <v>1.3943000000000001E-2</v>
-      </c>
-      <c r="L6" s="12">
-        <v>-11.305999999999999</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N6" s="8" t="s">
+      <c r="J6">
+        <v>-0.398752</v>
+      </c>
+      <c r="K6">
+        <v>2.3519999999999999E-2</v>
+      </c>
+      <c r="L6">
+        <v>-16.954000000000001</v>
+      </c>
+      <c r="M6" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="Q6" s="22">
+      <c r="Q6" s="21">
         <v>-1.67899</v>
       </c>
-      <c r="R6" s="22">
+      <c r="R6" s="21">
         <v>9.6310000000000007E-2</v>
       </c>
-      <c r="S6" s="22">
+      <c r="S6" s="21">
         <v>-17.434000000000001</v>
       </c>
-      <c r="T6" s="21" t="s">
+      <c r="T6" s="20" t="s">
         <v>425</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="Y6" s="12">
+      <c r="Y6" s="11">
         <v>-4.5236999999999999E-2</v>
       </c>
-      <c r="Z6" s="12">
+      <c r="Z6" s="11">
         <v>5.6309999999999997E-3</v>
       </c>
-      <c r="AA6" s="12">
+      <c r="AA6" s="11">
         <v>-8.0340000000000007</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AB6" s="12">
         <v>2.8200000000000001E-15</v>
       </c>
     </row>
@@ -13543,67 +13544,67 @@
       <c r="B7" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>-0.31301800000000002</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>1.5528E-2</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>-20.158000000000001</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="J7" s="12">
-        <v>-0.31301800000000002</v>
-      </c>
-      <c r="K7" s="13">
-        <v>1.5528E-2</v>
-      </c>
-      <c r="L7" s="12">
-        <v>-20.158000000000001</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N7" s="8" t="s">
+      <c r="J7">
+        <v>-0.554894</v>
+      </c>
+      <c r="K7">
+        <v>2.6695E-2</v>
+      </c>
+      <c r="L7">
+        <v>-20.786999999999999</v>
+      </c>
+      <c r="M7" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N7" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="21">
         <v>-2.6410999999999998</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="21">
         <v>9.7229999999999997E-2</v>
       </c>
-      <c r="S7" s="22">
+      <c r="S7" s="21">
         <v>-27.164999999999999</v>
       </c>
-      <c r="T7" s="21" t="s">
+      <c r="T7" s="20" t="s">
         <v>425</v>
       </c>
       <c r="X7" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="Y7" s="12">
+      <c r="Y7" s="11">
         <v>-8.2936999999999997E-2</v>
       </c>
-      <c r="Z7" s="12">
+      <c r="Z7" s="11">
         <v>5.7460000000000002E-3</v>
       </c>
-      <c r="AA7" s="12">
+      <c r="AA7" s="11">
         <v>-14.433999999999999</v>
       </c>
-      <c r="AB7" s="21" t="s">
+      <c r="AB7" s="20" t="s">
         <v>425</v>
       </c>
     </row>
@@ -13611,67 +13612,64 @@
       <c r="B8" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>4.3493999999999998E-2</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>1.1552E-2</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>3.7650000000000001</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>1.7699999999999999E-4</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="J8" s="13">
-        <v>4.3493999999999998E-2</v>
-      </c>
-      <c r="K8" s="13">
-        <v>1.1552E-2</v>
-      </c>
-      <c r="L8" s="12">
-        <v>3.7650000000000001</v>
-      </c>
-      <c r="M8" s="13">
-        <v>1.7699999999999999E-4</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>62</v>
+      <c r="J8">
+        <v>2.8739999999999998E-3</v>
+      </c>
+      <c r="K8">
+        <v>1.6996000000000001E-2</v>
+      </c>
+      <c r="L8">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="M8">
+        <v>0.86599999999999999</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="21">
         <v>9.8449999999999996E-2</v>
       </c>
-      <c r="R8" s="22">
+      <c r="R8" s="21">
         <v>8.8349999999999998E-2</v>
       </c>
-      <c r="S8" s="22">
+      <c r="S8" s="21">
         <v>1.1140000000000001</v>
       </c>
-      <c r="T8" s="22">
+      <c r="T8" s="21">
         <v>0.26500000000000001</v>
       </c>
       <c r="X8" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="Y8" s="12">
+      <c r="Y8" s="11">
         <v>4.7609999999999996E-3</v>
       </c>
-      <c r="Z8" s="12">
+      <c r="Z8" s="11">
         <v>5.0400000000000002E-3</v>
       </c>
-      <c r="AA8" s="12">
+      <c r="AA8" s="11">
         <v>0.94499999999999995</v>
       </c>
-      <c r="AB8" s="12">
+      <c r="AB8" s="11">
         <v>0.34511700000000001</v>
       </c>
     </row>
@@ -13679,61 +13677,61 @@
       <c r="B9" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>9.9410000000000002E-3</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>1.7724E-2</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>0.56100000000000005</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>0.57501500000000005</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="J9" s="13">
-        <v>9.9410000000000002E-3</v>
-      </c>
-      <c r="K9" s="13">
-        <v>1.7724E-2</v>
-      </c>
-      <c r="L9" s="12">
-        <v>0.56100000000000005</v>
-      </c>
-      <c r="M9" s="12">
-        <v>0.57501500000000005</v>
+      <c r="J9">
+        <v>-2.6131000000000001E-2</v>
+      </c>
+      <c r="K9">
+        <v>3.0678E-2</v>
+      </c>
+      <c r="L9">
+        <v>-0.85199999999999998</v>
+      </c>
+      <c r="M9">
+        <v>0.39500000000000002</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="Q9" s="21">
         <v>-0.25535000000000002</v>
       </c>
-      <c r="R9" s="22">
+      <c r="R9" s="21">
         <v>0.12479999999999999</v>
       </c>
-      <c r="S9" s="22">
+      <c r="S9" s="21">
         <v>-2.0459999999999998</v>
       </c>
-      <c r="T9" s="22">
+      <c r="T9" s="21">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="X9" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="Y9" s="12">
+      <c r="Y9" s="11">
         <v>-2.4868999999999999E-2</v>
       </c>
-      <c r="Z9" s="12">
+      <c r="Z9" s="11">
         <v>7.3429999999999997E-3</v>
       </c>
-      <c r="AA9" s="12">
+      <c r="AA9" s="11">
         <v>-3.387</v>
       </c>
-      <c r="AB9" s="14">
+      <c r="AB9" s="13">
         <v>7.3700000000000002E-4</v>
       </c>
     </row>
@@ -13741,69 +13739,69 @@
       <c r="B10" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>3.1896000000000001E-2</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>1.9782999999999999E-2</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>1.6120000000000001</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>0.107237</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="J10" s="13">
-        <v>3.1896000000000001E-2</v>
-      </c>
-      <c r="K10" s="13">
-        <v>1.9782999999999999E-2</v>
-      </c>
-      <c r="L10" s="12">
-        <v>1.6120000000000001</v>
-      </c>
-      <c r="M10" s="12">
-        <v>0.107237</v>
+      <c r="J10">
+        <v>-6.3879999999999996E-3</v>
+      </c>
+      <c r="K10">
+        <v>3.4980999999999998E-2</v>
+      </c>
+      <c r="L10">
+        <v>-0.183</v>
+      </c>
+      <c r="M10">
+        <v>0.85499999999999998</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="Q10" s="22">
+      <c r="Q10" s="21">
         <v>-0.11594</v>
       </c>
-      <c r="R10" s="22">
+      <c r="R10" s="21">
         <v>0.12684000000000001</v>
       </c>
-      <c r="S10" s="22">
+      <c r="S10" s="21">
         <v>-0.91400000000000003</v>
       </c>
-      <c r="T10" s="22">
+      <c r="T10" s="21">
         <v>0.36099999999999999</v>
       </c>
       <c r="X10" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="Y10" s="12">
+      <c r="Y10" s="11">
         <v>-5.2760000000000003E-3</v>
       </c>
-      <c r="Z10" s="12">
+      <c r="Z10" s="11">
         <v>7.541E-3</v>
       </c>
-      <c r="AA10" s="12">
+      <c r="AA10" s="11">
         <v>-0.7</v>
       </c>
-      <c r="AB10" s="12">
+      <c r="AB10" s="11">
         <v>0.48430499999999999</v>
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -13854,16 +13852,16 @@
       <c r="X12" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="Y12" s="23" t="s">
+      <c r="Y12" s="22" t="s">
         <v>618</v>
       </c>
-      <c r="Z12" s="23" t="s">
+      <c r="Z12" s="22" t="s">
         <v>619</v>
       </c>
-      <c r="AA12" s="23" t="s">
+      <c r="AA12" s="22" t="s">
         <v>620</v>
       </c>
-      <c r="AB12" s="23" t="s">
+      <c r="AB12" s="22" t="s">
         <v>621</v>
       </c>
     </row>
@@ -13871,67 +13869,67 @@
       <c r="B13" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>3.0078140000000002</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>8.1779999999999995E-3</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>367.78</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="J13" s="12">
-        <v>3.0078140000000002</v>
-      </c>
-      <c r="K13" s="13">
-        <v>8.1779999999999995E-3</v>
-      </c>
-      <c r="L13" s="12">
-        <v>367.78</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N13" s="8" t="s">
+      <c r="J13">
+        <v>1.1168610000000001</v>
+      </c>
+      <c r="K13">
+        <v>9.7669999999999996E-3</v>
+      </c>
+      <c r="L13">
+        <v>114.34699999999999</v>
+      </c>
+      <c r="M13" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N13" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="Q13" s="12">
+      <c r="Q13" s="11">
         <v>4.1160220000000001</v>
       </c>
-      <c r="R13" s="12">
+      <c r="R13" s="11">
         <v>6.0004000000000002E-2</v>
       </c>
-      <c r="S13" s="12">
+      <c r="S13" s="11">
         <v>68.596000000000004</v>
       </c>
-      <c r="T13" s="14" t="s">
+      <c r="T13" s="13" t="s">
         <v>425</v>
       </c>
       <c r="X13" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="Y13" s="12">
+      <c r="Y13" s="11">
         <v>1.0309026999999999</v>
       </c>
-      <c r="Z13" s="12">
+      <c r="Z13" s="11">
         <v>3.5241000000000001E-3</v>
       </c>
-      <c r="AA13" s="12">
+      <c r="AA13" s="11">
         <v>292.529</v>
       </c>
-      <c r="AB13" s="14" t="s">
+      <c r="AB13" s="13" t="s">
         <v>425</v>
       </c>
     </row>
@@ -13939,67 +13937,67 @@
       <c r="B14" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>-0.182947</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>1.2718E-2</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>-14.385</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="J14" s="12">
-        <v>-0.182947</v>
-      </c>
-      <c r="K14" s="13">
-        <v>1.2718E-2</v>
-      </c>
-      <c r="L14" s="12">
-        <v>-14.385</v>
-      </c>
-      <c r="M14" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N14" s="8" t="s">
+      <c r="J14">
+        <v>-0.46250000000000002</v>
+      </c>
+      <c r="K14">
+        <v>1.8223E-2</v>
+      </c>
+      <c r="L14">
+        <v>-25.38</v>
+      </c>
+      <c r="M14" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N14" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P14" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="11">
         <v>-1.338848</v>
       </c>
-      <c r="R14" s="12">
+      <c r="R14" s="11">
         <v>8.4511000000000003E-2</v>
       </c>
-      <c r="S14" s="12">
+      <c r="S14" s="11">
         <v>-15.842000000000001</v>
       </c>
-      <c r="T14" s="14" t="s">
+      <c r="T14" s="13" t="s">
         <v>425</v>
       </c>
       <c r="X14" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="Y14" s="12">
+      <c r="Y14" s="11">
         <v>-5.9019599999999998E-2</v>
       </c>
-      <c r="Z14" s="12">
+      <c r="Z14" s="11">
         <v>5.1224E-3</v>
       </c>
-      <c r="AA14" s="12">
+      <c r="AA14" s="11">
         <v>-11.522</v>
       </c>
-      <c r="AB14" s="14" t="s">
+      <c r="AB14" s="13" t="s">
         <v>425</v>
       </c>
     </row>
@@ -14007,67 +14005,67 @@
       <c r="B15" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>-0.25945200000000002</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>1.4531000000000001E-2</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>-17.855</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="J15" s="12">
-        <v>-0.25945200000000002</v>
-      </c>
-      <c r="K15" s="13">
-        <v>1.4531000000000001E-2</v>
-      </c>
-      <c r="L15" s="12">
-        <v>-17.855</v>
-      </c>
-      <c r="M15" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N15" s="8" t="s">
+      <c r="J15">
+        <v>-0.85613499999999998</v>
+      </c>
+      <c r="K15">
+        <v>2.7822E-2</v>
+      </c>
+      <c r="L15">
+        <v>-30.771999999999998</v>
+      </c>
+      <c r="M15" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N15" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P15" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="Q15" s="12">
+      <c r="Q15" s="11">
         <v>-2.3713410000000001</v>
       </c>
-      <c r="R15" s="12">
+      <c r="R15" s="11">
         <v>9.0676999999999994E-2</v>
       </c>
-      <c r="S15" s="12">
+      <c r="S15" s="11">
         <v>-26.152000000000001</v>
       </c>
-      <c r="T15" s="14" t="s">
+      <c r="T15" s="13" t="s">
         <v>425</v>
       </c>
       <c r="X15" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="Y15" s="12">
+      <c r="Y15" s="11">
         <v>-0.11669350000000001</v>
       </c>
-      <c r="Z15" s="12">
+      <c r="Z15" s="11">
         <v>5.7399E-3</v>
       </c>
-      <c r="AA15" s="12">
+      <c r="AA15" s="11">
         <v>-20.329999999999998</v>
       </c>
-      <c r="AB15" s="14" t="s">
+      <c r="AB15" s="13" t="s">
         <v>425</v>
       </c>
     </row>
@@ -14075,67 +14073,64 @@
       <c r="B16" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>5.8056999999999997E-2</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>1.1091999999999999E-2</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>5.234</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="J16" s="12">
-        <v>5.8056999999999997E-2</v>
-      </c>
-      <c r="K16" s="13">
-        <v>1.1091999999999999E-2</v>
-      </c>
-      <c r="L16" s="12">
-        <v>5.234</v>
-      </c>
-      <c r="M16" s="13">
-        <v>1.9999999999999999E-7</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>62</v>
+      <c r="J16">
+        <v>-1.1328E-2</v>
+      </c>
+      <c r="K16">
+        <v>1.3689E-2</v>
+      </c>
+      <c r="L16">
+        <v>-0.82799999999999996</v>
+      </c>
+      <c r="M16">
+        <v>0.40810000000000002</v>
       </c>
       <c r="P16" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="Q16" s="12">
+      <c r="Q16" s="11">
         <v>-1.439E-3</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="11">
         <v>8.3634E-2</v>
       </c>
-      <c r="S16" s="12">
+      <c r="S16" s="11">
         <v>-1.7000000000000001E-2</v>
       </c>
-      <c r="T16" s="12">
+      <c r="T16" s="11">
         <v>0.98629999999999995</v>
       </c>
       <c r="X16" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="Y16" s="12">
+      <c r="Y16" s="11">
         <v>9.2230000000000003E-4</v>
       </c>
-      <c r="Z16" s="12">
+      <c r="Z16" s="11">
         <v>4.9148999999999998E-3</v>
       </c>
-      <c r="AA16" s="12">
+      <c r="AA16" s="11">
         <v>0.188</v>
       </c>
-      <c r="AB16" s="12">
+      <c r="AB16" s="11">
         <v>0.85099999999999998</v>
       </c>
     </row>
@@ -14143,67 +14138,64 @@
       <c r="B17" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <v>-3.3419999999999998E-2</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>1.7385000000000001E-2</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>-1.9219999999999999</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>5.4826E-2</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>71</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="J17" s="12">
-        <v>-3.3419999999999998E-2</v>
-      </c>
-      <c r="K17" s="13">
-        <v>1.7385000000000001E-2</v>
-      </c>
-      <c r="L17" s="12">
-        <v>-1.9219999999999999</v>
-      </c>
-      <c r="M17" s="12">
-        <v>5.4826E-2</v>
-      </c>
-      <c r="N17" s="8" t="s">
-        <v>71</v>
+      <c r="J17">
+        <v>8.6580000000000008E-3</v>
+      </c>
+      <c r="K17">
+        <v>2.5422E-2</v>
+      </c>
+      <c r="L17">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="M17">
+        <v>0.73350000000000004</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="Q17" s="12">
+      <c r="Q17" s="11">
         <v>0.22934099999999999</v>
       </c>
-      <c r="R17" s="12">
+      <c r="R17" s="11">
         <v>0.117662</v>
       </c>
-      <c r="S17" s="12">
+      <c r="S17" s="11">
         <v>1.9490000000000001</v>
       </c>
-      <c r="T17" s="12">
+      <c r="T17" s="11">
         <v>5.1499999999999997E-2</v>
       </c>
       <c r="X17" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="Y17" s="12">
+      <c r="Y17" s="11">
         <v>2.6613000000000001E-3</v>
       </c>
-      <c r="Z17" s="12">
+      <c r="Z17" s="11">
         <v>7.1301999999999997E-3</v>
       </c>
-      <c r="AA17" s="12">
+      <c r="AA17" s="11">
         <v>0.373</v>
       </c>
-      <c r="AB17" s="12">
+      <c r="AB17" s="11">
         <v>0.70899999999999996</v>
       </c>
     </row>
@@ -14211,75 +14203,75 @@
       <c r="B18" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>-6.8000000000000005E-2</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>1.9924000000000001E-2</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>-3.4129999999999998</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>6.6699999999999995E-4</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="J18" s="12">
-        <v>-6.8000000000000005E-2</v>
-      </c>
-      <c r="K18" s="13">
-        <v>1.9924000000000001E-2</v>
-      </c>
-      <c r="L18" s="12">
-        <v>-3.4129999999999998</v>
-      </c>
-      <c r="M18" s="13">
-        <v>6.6699999999999995E-4</v>
-      </c>
-      <c r="N18" s="8" t="s">
-        <v>62</v>
+      <c r="J18">
+        <v>9.1528999999999999E-2</v>
+      </c>
+      <c r="K18">
+        <v>3.7087000000000002E-2</v>
+      </c>
+      <c r="L18">
+        <v>2.468</v>
+      </c>
+      <c r="M18" s="89">
+        <v>1.37E-2</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="Q18" s="12">
+      <c r="Q18" s="11">
         <v>-1.8242000000000001E-2</v>
       </c>
-      <c r="R18" s="12">
+      <c r="R18" s="11">
         <v>0.12525700000000001</v>
       </c>
-      <c r="S18" s="12">
+      <c r="S18" s="11">
         <v>-0.14599999999999999</v>
       </c>
-      <c r="T18" s="12">
+      <c r="T18" s="11">
         <v>0.88419999999999999</v>
       </c>
       <c r="X18" s="6" t="s">
         <v>634</v>
       </c>
-      <c r="Y18" s="12">
+      <c r="Y18" s="11">
         <v>9.1874999999999995E-3</v>
       </c>
-      <c r="Z18" s="12">
+      <c r="Z18" s="11">
         <v>7.8951999999999998E-3</v>
       </c>
-      <c r="AA18" s="12">
+      <c r="AA18" s="11">
         <v>1.1639999999999999</v>
       </c>
-      <c r="AB18" s="12">
+      <c r="AB18" s="11">
         <v>0.245</v>
       </c>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
@@ -14330,16 +14322,16 @@
       <c r="X20" s="4" t="s">
         <v>635</v>
       </c>
-      <c r="Y20" s="23" t="s">
+      <c r="Y20" s="22" t="s">
         <v>618</v>
       </c>
-      <c r="Z20" s="23" t="s">
+      <c r="Z20" s="22" t="s">
         <v>619</v>
       </c>
-      <c r="AA20" s="23" t="s">
+      <c r="AA20" s="22" t="s">
         <v>620</v>
       </c>
-      <c r="AB20" s="23" t="s">
+      <c r="AB20" s="22" t="s">
         <v>621</v>
       </c>
     </row>
@@ -14347,67 +14339,67 @@
       <c r="B21" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>3.0543089999999999</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>1.1594999999999999E-2</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>263.41899999999998</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="J21" s="12">
-        <v>3.0543089999999999</v>
-      </c>
-      <c r="K21" s="13">
-        <v>1.1594999999999999E-2</v>
-      </c>
-      <c r="L21" s="12">
-        <v>263.41899999999998</v>
-      </c>
-      <c r="M21" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N21" s="8" t="s">
+      <c r="J21">
+        <v>0.92495000000000005</v>
+      </c>
+      <c r="K21">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="L21">
+        <v>50.820999999999998</v>
+      </c>
+      <c r="M21" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N21" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P21" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="Q21" s="12">
+      <c r="Q21" s="11">
         <v>3.46739</v>
       </c>
-      <c r="R21" s="12">
+      <c r="R21" s="11">
         <v>6.6019999999999995E-2</v>
       </c>
-      <c r="S21" s="12">
+      <c r="S21" s="11">
         <v>52.518999999999998</v>
       </c>
-      <c r="T21" s="14" t="s">
+      <c r="T21" s="13" t="s">
         <v>425</v>
       </c>
       <c r="X21" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="Y21" s="12">
+      <c r="Y21" s="11">
         <v>1.022661</v>
       </c>
-      <c r="Z21" s="12">
+      <c r="Z21" s="11">
         <v>4.6639999999999997E-3</v>
       </c>
-      <c r="AA21" s="12">
+      <c r="AA21" s="11">
         <v>219.27</v>
       </c>
-      <c r="AB21" s="14" t="s">
+      <c r="AB21" s="13" t="s">
         <v>425</v>
       </c>
     </row>
@@ -14415,67 +14407,67 @@
       <c r="B22" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <v>-0.102379</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>1.7752E-2</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>-5.7670000000000003</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="14">
         <v>1.85E-8</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="J22" s="12">
-        <v>-0.102379</v>
-      </c>
-      <c r="K22" s="13">
-        <v>1.7752E-2</v>
-      </c>
-      <c r="L22" s="12">
-        <v>-5.7670000000000003</v>
-      </c>
-      <c r="M22" s="13">
-        <v>1.85E-8</v>
-      </c>
-      <c r="N22" s="8" t="s">
+      <c r="J22">
+        <v>-0.31234000000000001</v>
+      </c>
+      <c r="K22">
+        <v>3.1759999999999997E-2</v>
+      </c>
+      <c r="L22">
+        <v>-9.8339999999999996</v>
+      </c>
+      <c r="M22" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N22" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="Q22" s="12">
+      <c r="Q22" s="11">
         <v>-1.16977</v>
       </c>
-      <c r="R22" s="12">
+      <c r="R22" s="11">
         <v>9.5570000000000002E-2</v>
       </c>
-      <c r="S22" s="12">
+      <c r="S22" s="11">
         <v>-12.241</v>
       </c>
-      <c r="T22" s="14" t="s">
+      <c r="T22" s="13" t="s">
         <v>425</v>
       </c>
       <c r="X22" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="Y22" s="12">
+      <c r="Y22" s="11">
         <v>-2.8965000000000001E-2</v>
       </c>
-      <c r="Z22" s="12">
+      <c r="Z22" s="11">
         <v>6.8840000000000004E-3</v>
       </c>
-      <c r="AA22" s="12">
+      <c r="AA22" s="11">
         <v>-4.2069999999999999</v>
       </c>
-      <c r="AB22" s="13">
+      <c r="AB22" s="12">
         <v>3.3599999999999997E-5</v>
       </c>
     </row>
@@ -14483,67 +14475,67 @@
       <c r="B23" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>-0.209563</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>1.9983999999999998E-2</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>-10.487</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="J23" s="12">
-        <v>-0.209563</v>
-      </c>
-      <c r="K23" s="13">
-        <v>1.9983999999999998E-2</v>
-      </c>
-      <c r="L23" s="12">
-        <v>-10.487</v>
-      </c>
-      <c r="M23" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N23" s="8" t="s">
+      <c r="J23">
+        <v>-0.78090999999999999</v>
+      </c>
+      <c r="K23">
+        <v>4.8759999999999998E-2</v>
+      </c>
+      <c r="L23">
+        <v>-16.015999999999998</v>
+      </c>
+      <c r="M23" s="89" t="s">
+        <v>425</v>
+      </c>
+      <c r="N23" s="7" t="s">
         <v>62</v>
       </c>
       <c r="P23" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="Q23" s="12">
+      <c r="Q23" s="11">
         <v>-1.6927399999999999</v>
       </c>
-      <c r="R23" s="12">
+      <c r="R23" s="11">
         <v>0.10002999999999999</v>
       </c>
-      <c r="S23" s="12">
+      <c r="S23" s="11">
         <v>-16.922000000000001</v>
       </c>
-      <c r="T23" s="14" t="s">
+      <c r="T23" s="13" t="s">
         <v>425</v>
       </c>
       <c r="X23" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="Y23" s="12">
+      <c r="Y23" s="11">
         <v>-8.4042000000000006E-2</v>
       </c>
-      <c r="Z23" s="12">
+      <c r="Z23" s="11">
         <v>7.4130000000000003E-3</v>
       </c>
-      <c r="AA23" s="12">
+      <c r="AA23" s="11">
         <v>-11.337999999999999</v>
       </c>
-      <c r="AB23" s="14" t="s">
+      <c r="AB23" s="13" t="s">
         <v>425</v>
       </c>
     </row>
@@ -14551,61 +14543,61 @@
       <c r="B24" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>1.8095E-2</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>2.2522E-2</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>0.80300000000000005</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <v>0.42230000000000001</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="J24" s="12">
-        <v>1.8095E-2</v>
-      </c>
-      <c r="K24" s="13">
-        <v>2.2522E-2</v>
-      </c>
-      <c r="L24" s="12">
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="M24" s="12">
-        <v>0.42230000000000001</v>
+      <c r="J24">
+        <v>4.0129999999999999E-2</v>
+      </c>
+      <c r="K24">
+        <v>3.4790000000000001E-2</v>
+      </c>
+      <c r="L24">
+        <v>1.1539999999999999</v>
+      </c>
+      <c r="M24">
+        <v>0.249</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="Q24" s="12">
+      <c r="Q24" s="11">
         <v>9.511E-2</v>
       </c>
-      <c r="R24" s="12">
+      <c r="R24" s="11">
         <v>0.12995999999999999</v>
       </c>
-      <c r="S24" s="12">
+      <c r="S24" s="11">
         <v>0.73199999999999998</v>
       </c>
-      <c r="T24" s="12">
+      <c r="T24" s="11">
         <v>0.46500000000000002</v>
       </c>
       <c r="X24" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="Y24" s="12">
+      <c r="Y24" s="11">
         <v>2.2040000000000001E-2</v>
       </c>
-      <c r="Z24" s="12">
+      <c r="Z24" s="11">
         <v>9.0279999999999996E-3</v>
       </c>
-      <c r="AA24" s="12">
+      <c r="AA24" s="11">
         <v>2.4409999999999998</v>
       </c>
-      <c r="AB24" s="12">
+      <c r="AB24" s="11">
         <v>1.52E-2</v>
       </c>
     </row>
@@ -14613,61 +14605,61 @@
       <c r="B25" s="6" t="s">
         <v>638</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <v>8.4159999999999999E-3</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>3.3154000000000003E-2</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>0.254</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="8">
         <v>0.79979999999999996</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>638</v>
       </c>
-      <c r="J25" s="12">
-        <v>8.4159999999999999E-3</v>
-      </c>
-      <c r="K25" s="13">
-        <v>3.3154000000000003E-2</v>
-      </c>
-      <c r="L25" s="12">
-        <v>0.254</v>
-      </c>
-      <c r="M25" s="12">
-        <v>0.79979999999999996</v>
+      <c r="J25">
+        <v>-4.9209999999999997E-2</v>
+      </c>
+      <c r="K25">
+        <v>5.953E-2</v>
+      </c>
+      <c r="L25">
+        <v>-0.82699999999999996</v>
+      </c>
+      <c r="M25">
+        <v>0.40899999999999997</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>638</v>
       </c>
-      <c r="Q25" s="12">
+      <c r="Q25" s="11">
         <v>3.5839999999999997E-2</v>
       </c>
-      <c r="R25" s="12">
+      <c r="R25" s="11">
         <v>0.18199000000000001</v>
       </c>
-      <c r="S25" s="12">
+      <c r="S25" s="11">
         <v>0.19700000000000001</v>
       </c>
-      <c r="T25" s="12">
+      <c r="T25" s="11">
         <v>0.84399999999999997</v>
       </c>
       <c r="X25" s="6" t="s">
         <v>638</v>
       </c>
-      <c r="Y25" s="12">
+      <c r="Y25" s="11">
         <v>1.0718E-2</v>
       </c>
-      <c r="Z25" s="12">
+      <c r="Z25" s="11">
         <v>1.286E-2</v>
       </c>
-      <c r="AA25" s="12">
+      <c r="AA25" s="11">
         <v>0.83299999999999996</v>
       </c>
-      <c r="AB25" s="12">
+      <c r="AB25" s="11">
         <v>0.4052</v>
       </c>
     </row>
@@ -14675,75 +14667,72 @@
       <c r="B26" s="6" t="s">
         <v>639</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8">
         <v>6.8352999999999997E-2</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="9">
         <v>3.7832999999999999E-2</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>1.8069999999999999</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="8">
         <v>7.17E-2</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>71</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>639</v>
       </c>
-      <c r="J26" s="12">
-        <v>6.8352999999999997E-2</v>
-      </c>
-      <c r="K26" s="13">
-        <v>3.7832999999999999E-2</v>
-      </c>
-      <c r="L26" s="12">
-        <v>1.8069999999999999</v>
-      </c>
-      <c r="M26" s="12">
-        <v>7.17E-2</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>71</v>
+      <c r="J26">
+        <v>-6.6390000000000005E-2</v>
+      </c>
+      <c r="K26">
+        <v>9.8159999999999997E-2</v>
+      </c>
+      <c r="L26">
+        <v>-0.67600000000000005</v>
+      </c>
+      <c r="M26">
+        <v>0.499</v>
       </c>
       <c r="P26" s="6" t="s">
         <v>639</v>
       </c>
-      <c r="Q26" s="12">
+      <c r="Q26" s="11">
         <v>0.21357999999999999</v>
       </c>
-      <c r="R26" s="12">
+      <c r="R26" s="11">
         <v>0.19811000000000001</v>
       </c>
-      <c r="S26" s="12">
+      <c r="S26" s="11">
         <v>1.0780000000000001</v>
       </c>
-      <c r="T26" s="12">
+      <c r="T26" s="11">
         <v>0.28199999999999997</v>
       </c>
       <c r="X26" s="6" t="s">
         <v>639</v>
       </c>
-      <c r="Y26" s="12">
+      <c r="Y26" s="11">
         <v>2.2963000000000001E-2</v>
       </c>
-      <c r="Z26" s="12">
+      <c r="Z26" s="11">
         <v>1.421E-2</v>
       </c>
-      <c r="AA26" s="12">
+      <c r="AA26" s="11">
         <v>1.6160000000000001</v>
       </c>
-      <c r="AB26" s="12">
+      <c r="AB26" s="11">
         <v>0.1071</v>
       </c>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="14"/>
-      <c r="AB27" s="14"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="13"/>
+      <c r="AB27" s="13"/>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
@@ -14762,7 +14751,7 @@
         <v>621</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>618</v>
@@ -14794,16 +14783,16 @@
       <c r="X28" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="Y28" s="23" t="s">
+      <c r="Y28" s="22" t="s">
         <v>618</v>
       </c>
-      <c r="Z28" s="23" t="s">
+      <c r="Z28" s="22" t="s">
         <v>619</v>
       </c>
-      <c r="AA28" s="23" t="s">
+      <c r="AA28" s="22" t="s">
         <v>620</v>
       </c>
-      <c r="AB28" s="23" t="s">
+      <c r="AB28" s="22" t="s">
         <v>621</v>
       </c>
     </row>
@@ -14811,67 +14800,56 @@
       <c r="B29" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="15">
         <v>3.15</v>
       </c>
-      <c r="D29" s="16">
+      <c r="D29" s="15">
         <v>3.3529999999999997E-2</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="16">
         <v>93.944000000000003</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="17">
         <v>2E-16</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="J29" s="12">
-        <v>3.1591399999999998</v>
-      </c>
-      <c r="K29" s="13">
-        <v>1.031E-2</v>
-      </c>
-      <c r="L29" s="12">
-        <v>306.56</v>
-      </c>
-      <c r="M29" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="J29" s="11"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="13"/>
       <c r="P29" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="Q29" s="12">
+      <c r="Q29" s="11">
         <v>4.8</v>
       </c>
-      <c r="R29" s="12">
+      <c r="R29" s="11">
         <v>0.20813000000000001</v>
       </c>
-      <c r="S29" s="12">
+      <c r="S29" s="11">
         <v>23.062000000000001</v>
       </c>
-      <c r="T29" s="11" t="s">
+      <c r="T29" s="10" t="s">
         <v>629</v>
       </c>
       <c r="X29" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="Y29" s="12">
+      <c r="Y29" s="11">
         <v>1.0675589999999999</v>
       </c>
-      <c r="Z29" s="12">
+      <c r="Z29" s="11">
         <v>1.1812E-2</v>
       </c>
-      <c r="AA29" s="12">
+      <c r="AA29" s="11">
         <v>90.376000000000005</v>
       </c>
-      <c r="AB29" s="14" t="s">
+      <c r="AB29" s="13" t="s">
         <v>425</v>
       </c>
     </row>
@@ -14879,67 +14857,56 @@
       <c r="B30" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="15">
         <v>-0.25209999999999999</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="15">
         <v>5.1119999999999999E-2</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="16">
         <v>-4.9320000000000004</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="17">
         <v>1.4699999999999999E-6</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="J30" s="12">
-        <v>-0.20152999999999999</v>
-      </c>
-      <c r="K30" s="13">
-        <v>-1.652E-2</v>
-      </c>
-      <c r="L30" s="12">
-        <v>-12.2</v>
-      </c>
-      <c r="M30" s="13">
-        <v>1.85E-8</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="J30" s="11"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="12"/>
       <c r="P30" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="Q30" s="12">
+      <c r="Q30" s="11">
         <v>-1.8714299999999999</v>
       </c>
-      <c r="R30" s="12">
+      <c r="R30" s="11">
         <v>0.27250999999999997</v>
       </c>
-      <c r="S30" s="12">
+      <c r="S30" s="11">
         <v>-6.867</v>
       </c>
-      <c r="T30" s="13">
+      <c r="T30" s="12">
         <v>2.78E-11</v>
       </c>
       <c r="X30" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="Y30" s="12">
+      <c r="Y30" s="11">
         <v>-5.8819999999999997E-2</v>
       </c>
-      <c r="Z30" s="12">
+      <c r="Z30" s="11">
         <v>1.6213000000000002E-2</v>
       </c>
-      <c r="AA30" s="12">
+      <c r="AA30" s="11">
         <v>-3.6280000000000001</v>
       </c>
-      <c r="AB30" s="13">
+      <c r="AB30" s="12">
         <v>3.4699999999999998E-4</v>
       </c>
     </row>
@@ -14947,77 +14914,66 @@
       <c r="B31" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="15">
         <v>-0.33150000000000002</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D31" s="15">
         <v>8.7569999999999995E-2</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="16">
         <v>-3.7850000000000001</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="19">
         <v>1.92E-4</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="7" t="s">
         <v>62</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="J31" s="12">
-        <v>-0.33849000000000001</v>
-      </c>
-      <c r="K31" s="13">
-        <v>-3.0380000000000001E-2</v>
-      </c>
-      <c r="L31" s="12">
-        <v>-11.14</v>
-      </c>
-      <c r="M31" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="N31" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="13"/>
       <c r="P31" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="Q31" s="12">
+      <c r="Q31" s="11">
         <v>-2.7285699999999999</v>
       </c>
-      <c r="R31" s="12">
+      <c r="R31" s="11">
         <v>0.27250999999999997</v>
       </c>
-      <c r="S31" s="12">
+      <c r="S31" s="11">
         <v>-10.013</v>
       </c>
-      <c r="T31" s="11" t="s">
+      <c r="T31" s="10" t="s">
         <v>629</v>
       </c>
       <c r="X31" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="Y31" s="12">
+      <c r="Y31" s="11">
         <v>-8.2863000000000006E-2</v>
       </c>
-      <c r="Z31" s="12">
+      <c r="Z31" s="11">
         <v>2.4340000000000001E-2</v>
       </c>
-      <c r="AA31" s="12">
+      <c r="AA31" s="11">
         <v>-3.4039999999999999</v>
       </c>
-      <c r="AB31" s="13">
+      <c r="AB31" s="12">
         <v>7.7399999999999995E-4</v>
       </c>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -25704,8 +25660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B140" sqref="B140:E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27849,7 +27805,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N551"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A460" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>